<commit_message>
cancel is_techical choices in db
</commit_message>
<xml_diff>
--- a/Humanitarian_VS_Technical/Data/Professions/11 Офисные службы.xlsx
+++ b/Humanitarian_VS_Technical/Data/Professions/11 Офисные службы.xlsx
@@ -682,11 +682,7 @@
           <t>Делопроизводитель</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Гуманитарный</t>
-        </is>
-      </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3" ht="12.75" customHeight="1" s="42">
       <c r="A3" s="3" t="n">
@@ -715,6 +711,7 @@
           <t>Офис-менеджер</t>
         </is>
       </c>
+      <c r="G3" t="inlineStr"/>
     </row>
     <row r="4" ht="12.75" customHeight="1" s="42">
       <c r="A4" s="3" t="n">
@@ -743,6 +740,7 @@
           <t>Секретарь</t>
         </is>
       </c>
+      <c r="G4" t="inlineStr"/>
     </row>
     <row r="5" ht="12.75" customHeight="1" s="42">
       <c r="A5" s="3" t="n">
@@ -771,6 +769,7 @@
           <t>Бизнес-ассистент</t>
         </is>
       </c>
+      <c r="G5" t="inlineStr"/>
     </row>
     <row r="6" ht="12.75" customHeight="1" s="42">
       <c r="A6" s="3" t="n">
@@ -799,6 +798,7 @@
           <t>Заведующий канцелярией</t>
         </is>
       </c>
+      <c r="G6" t="inlineStr"/>
     </row>
     <row r="7" ht="12.75" customHeight="1" s="42">
       <c r="A7" s="3" t="n">
@@ -827,6 +827,7 @@
           <t>Менеджер по оформлению документов</t>
         </is>
       </c>
+      <c r="G7" t="inlineStr"/>
     </row>
     <row r="8" ht="12.75" customHeight="1" s="42">
       <c r="A8" s="3" t="n">
@@ -855,6 +856,7 @@
           <t>Стенографист</t>
         </is>
       </c>
+      <c r="G8" t="inlineStr"/>
     </row>
     <row r="9" ht="12.75" customHeight="1" s="42">
       <c r="A9" s="3" t="n">
@@ -883,6 +885,7 @@
           <t>Оператор Call-центра</t>
         </is>
       </c>
+      <c r="G9" t="inlineStr"/>
     </row>
     <row r="10" ht="12.75" customHeight="1" s="42">
       <c r="A10" s="3" t="n">
@@ -911,6 +914,7 @@
           <t>Консультант call-центра</t>
         </is>
       </c>
+      <c r="G10" t="inlineStr"/>
     </row>
     <row r="11" ht="12.75" customHeight="1" s="42">
       <c r="A11" s="3" t="n">
@@ -939,6 +943,7 @@
           <t>Архивист</t>
         </is>
       </c>
+      <c r="G11" t="inlineStr"/>
     </row>
     <row r="12" ht="12.75" customHeight="1" s="42">
       <c r="A12" s="3" t="n"/>

</xml_diff>